<commit_message>
updated blueprintfiles and reporttemplate
</commit_message>
<xml_diff>
--- a/templates/IssueBluePrintPilot.xlsx
+++ b/templates/IssueBluePrintPilot.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephankuche/CreateJiraIssues/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E3B58A-71CD-5C4F-A4E1-6A65DBF054D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063974FC-9EDE-F346-A7CD-3FB14ED05F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="4600" windowWidth="35300" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7140" yWindow="500" windowWidth="25600" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$172</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="210">
   <si>
     <t>Summary</t>
   </si>
@@ -660,6 +663,9 @@
   </si>
   <si>
     <t>MileStone_Hypercare Closing_Handover to Customer Care</t>
+  </si>
+  <si>
+    <t>Data Acquisition,Requirement Analysis</t>
   </si>
 </sst>
 </file>
@@ -834,567 +840,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="214">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="158">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3272,11 +2718,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F728FE19-0465-1C4B-A5E0-C11743CC7188}">
-  <dimension ref="A1:G187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD5E05C-EBFE-384E-9214-D4F9000DB306}">
+  <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3324,10 +2770,10 @@
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -3339,86 +2785,76 @@
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4">
-        <v>5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>154</v>
+      <c r="A5" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>65</v>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="3" t="s">
-        <v>155</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>156</v>
+      <c r="A6" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="3" t="s">
-        <v>155</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>67</v>
+      <c r="A7" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>65</v>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -3426,31 +2862,31 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>70</v>
+      <c r="A9" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>72</v>
+      <c r="A10" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>65</v>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3459,47 +2895,43 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>65</v>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -3507,23 +2939,29 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>75</v>
+      <c r="A14" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="2" t="s">
+        <v>209</v>
+      </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>76</v>
+      <c r="A15" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
@@ -3533,14 +2971,14 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>77</v>
+      <c r="F15" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>78</v>
+      <c r="A16" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
@@ -3550,12 +2988,14 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>79</v>
+      <c r="A17" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
@@ -3565,12 +3005,14 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
@@ -3584,8 +3026,8 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>81</v>
+      <c r="A19" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
@@ -3596,13 +3038,13 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>82</v>
+      <c r="A20" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
@@ -3617,7 +3059,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
@@ -3628,13 +3070,13 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
@@ -3644,12 +3086,14 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>86</v>
+      <c r="A23" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
@@ -3663,8 +3107,8 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>87</v>
+      <c r="A24" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
@@ -3678,8 +3122,8 @@
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>88</v>
+      <c r="A25" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
@@ -3690,13 +3134,13 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>155</v>
+        <v>77</v>
       </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>89</v>
+      <c r="A26" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>9</v>
@@ -3706,14 +3150,12 @@
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>90</v>
+      <c r="A27" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>9</v>
@@ -3723,14 +3165,12 @@
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>9</v>
@@ -3740,14 +3180,12 @@
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>160</v>
+      <c r="A29" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>9</v>
@@ -3758,13 +3196,13 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>91</v>
+      <c r="A30" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>9</v>
@@ -3778,8 +3216,8 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>92</v>
+      <c r="A31" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>9</v>
@@ -3789,12 +3227,14 @@
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>93</v>
+      <c r="A32" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>9</v>
@@ -3809,30 +3249,28 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>162</v>
+        <v>86</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4">
-        <v>1</v>
-      </c>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>153</v>
+      <c r="A34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -3841,186 +3279,186 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4">
-        <v>19</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="2"/>
+      <c r="F36" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="2" t="s">
-        <v>98</v>
+      <c r="F37" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>99</v>
+      <c r="A38" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="2"/>
+      <c r="F38" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>100</v>
+      <c r="A39" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>101</v>
+      <c r="A40" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>103</v>
+      <c r="A41" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>104</v>
+      <c r="A42" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>66</v>
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>66</v>
+      <c r="A44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
-      <c r="F44" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>9</v>
@@ -4035,7 +3473,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>9</v>
@@ -4046,13 +3484,13 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="2" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>166</v>
+        <v>99</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>9</v>
@@ -4067,7 +3505,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>9</v>
@@ -4082,7 +3520,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>9</v>
@@ -4092,205 +3530,191 @@
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
-      <c r="F50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>113</v>
+      <c r="A53" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="F53" s="2"/>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>114</v>
+      <c r="A54" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
-      <c r="F54" s="1" t="s">
-        <v>115</v>
+      <c r="F54" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>116</v>
+      <c r="A55" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="F55" s="2"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="F56" s="2"/>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>119</v>
+      <c r="A57" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="1" t="s">
-        <v>120</v>
+      <c r="F57" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
-      <c r="F58" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="F58" s="2"/>
       <c r="G58" s="4"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>122</v>
+      <c r="A59" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
-      <c r="F59" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="F59" s="2"/>
       <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>124</v>
+      <c r="A60" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F60" s="2"/>
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>125</v>
+      <c r="A61" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
+      <c r="E61" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
+      <c r="G61" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>9</v>
@@ -4300,14 +3724,14 @@
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="4" t="s">
-        <v>172</v>
+      <c r="F62" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>9</v>
@@ -4317,14 +3741,14 @@
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
-        <v>174</v>
+      <c r="F63" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>9</v>
@@ -4334,14 +3758,14 @@
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
-      <c r="F64" s="4" t="s">
-        <v>174</v>
+      <c r="F64" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>127</v>
+      <c r="A65" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>9</v>
@@ -4351,12 +3775,14 @@
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
+      <c r="F65" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>9</v>
@@ -4366,69 +3792,71 @@
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+      <c r="F66" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="G66" s="4"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>153</v>
+      <c r="A67" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
+      <c r="F67" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>112</v>
+      <c r="A68" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>130</v>
+      <c r="A69" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
+      <c r="F69" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="G69" s="4"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -4437,75 +3865,79 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="F71" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="G71" s="4"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
+      <c r="F72" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="G72" s="4"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>134</v>
+      <c r="A73" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
+      <c r="F73" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="G73" s="4"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
-      <c r="F74" s="1" t="s">
-        <v>177</v>
-      </c>
+      <c r="F74" s="4"/>
       <c r="G74" s="4"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -4513,29 +3945,35 @@
       <c r="G75" s="4"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>178</v>
+      <c r="A76" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
+      <c r="G76" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>112</v>
+        <v>129</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -4543,23 +3981,29 @@
       <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>137</v>
+      <c r="A78" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C78" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
+      <c r="E78" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
+      <c r="G78" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>9</v>
@@ -4574,7 +4018,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>9</v>
@@ -4589,7 +4033,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>9</v>
@@ -4603,8 +4047,8 @@
       <c r="G81" s="4"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>140</v>
+      <c r="A82" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>9</v>
@@ -4618,8 +4062,8 @@
       <c r="G82" s="4"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>151</v>
+      <c r="A83" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>9</v>
@@ -4633,8 +4077,8 @@
       <c r="G83" s="4"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>181</v>
+      <c r="A84" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>9</v>
@@ -4644,39 +4088,35 @@
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
+      <c r="F84" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="G84" s="4"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>176</v>
+      <c r="A85" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>182</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="4">
-        <v>1</v>
-      </c>
+      <c r="G85" s="4"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>153</v>
+      <c r="A86" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -4685,30 +4125,28 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>3</v>
+        <v>179</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D87" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="D87" s="4"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
-      <c r="G87" s="4">
-        <v>21</v>
-      </c>
+      <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>11</v>
+      <c r="A88" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>183</v>
+      <c r="C88" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -4717,13 +4155,13 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>183</v>
+      <c r="C89" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -4731,14 +4169,14 @@
       <c r="G89" s="4"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>13</v>
+      <c r="A90" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>183</v>
+      <c r="C90" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -4746,14 +4184,14 @@
       <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>14</v>
+      <c r="A91" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>183</v>
+      <c r="C91" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -4762,13 +4200,13 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>183</v>
+      <c r="C92" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -4776,14 +4214,14 @@
       <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>16</v>
+      <c r="A93" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>183</v>
+      <c r="C93" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -4791,14 +4229,14 @@
       <c r="G93" s="4"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>17</v>
+      <c r="A94" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>183</v>
+      <c r="C94" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -4806,31 +4244,35 @@
       <c r="G94" s="4"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B95" s="5" t="s">
+      <c r="A95" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D95" s="1"/>
-      <c r="E95" s="4"/>
+      <c r="C95" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>184</v>
+        <v>10</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -4838,29 +4280,31 @@
       <c r="G96" s="4"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D97" s="4"/>
+      <c r="A97" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
+      <c r="G97" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>143</v>
+        <v>11</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -4869,13 +4313,13 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -4884,13 +4328,13 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>153</v>
+        <v>13</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -4898,31 +4342,29 @@
       <c r="G100" s="4"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
+      <c r="A101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="G101" s="4">
-        <v>3</v>
-      </c>
+      <c r="G101" s="4"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>58</v>
+      <c r="A102" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -4930,14 +4372,14 @@
       <c r="G102" s="4"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>20</v>
+      <c r="A103" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -4946,62 +4388,60 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B104" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D105" s="4"/>
+      <c r="C105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
+      <c r="G105" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
+      <c r="A106" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="G106" s="4">
-        <v>2</v>
-      </c>
+      <c r="G106" s="4"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -5009,31 +4449,29 @@
       <c r="G107" s="4"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="1"/>
+      <c r="A108" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D108" s="4"/>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
-      <c r="G108" s="4">
-        <v>2</v>
-      </c>
+      <c r="G108" s="4"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>22</v>
+        <v>145</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -5041,46 +4479,46 @@
       <c r="G109" s="4"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>19</v>
+      <c r="A110" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="4">
-        <v>1</v>
-      </c>
+      <c r="G110" s="4"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
+      <c r="A111" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
       <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
+      <c r="G111" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>153</v>
+      <c r="A112" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -5088,114 +4526,110 @@
       <c r="G112" s="4"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>25</v>
+      <c r="A113" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
-      <c r="G113" s="4">
-        <v>1</v>
-      </c>
+      <c r="G113" s="4"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G114" s="4"/>
+      <c r="A114" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
-      <c r="F115" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="F115" s="4"/>
       <c r="G115" s="4"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G116" s="4"/>
+      <c r="A116" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>25</v>
+      <c r="A117" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
-      <c r="G117" s="4">
-        <v>14</v>
-      </c>
+      <c r="G117" s="4"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D118" s="4"/>
+        <v>188</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
-      <c r="G118" s="4"/>
+      <c r="G118" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>60</v>
+      <c r="A119" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>26</v>
+        <v>188</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -5204,49 +4638,45 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
+      <c r="G120" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E121" s="12" t="s">
-        <v>148</v>
-      </c>
+      <c r="A121" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
       <c r="F121" s="4"/>
-      <c r="G121" s="4">
-        <v>7</v>
-      </c>
+      <c r="G121" s="4"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -5254,89 +4684,103 @@
       <c r="G122" s="4"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>28</v>
+      <c r="A123" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
+      <c r="G123" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
+      <c r="F124" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="G124" s="4"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
-      <c r="F125" s="4"/>
+      <c r="F125" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="G125" s="4"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
+      <c r="F126" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="G126" s="4"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D127" s="4"/>
-      <c r="E127" s="4"/>
+      <c r="A127" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E127" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="F127" s="4"/>
-      <c r="G127" s="4"/>
+      <c r="G127" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>31</v>
+      <c r="A128" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -5344,14 +4788,14 @@
       <c r="G128" s="4"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="2" t="s">
-        <v>32</v>
+      <c r="A129" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -5359,14 +4803,14 @@
       <c r="G129" s="4"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="13" t="s">
-        <v>35</v>
+      <c r="A130" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -5374,67 +4818,61 @@
       <c r="G130" s="4"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B131" s="5" t="s">
+      <c r="A131" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131" s="1"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4">
         <v>7</v>
       </c>
-      <c r="C131" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="D131" s="4"/>
-      <c r="E131" s="4"/>
-      <c r="F131" s="4"/>
-      <c r="G131" s="4"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C132" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A132" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="G132" s="4">
-        <v>3</v>
-      </c>
+      <c r="G132" s="4"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
-      <c r="F133" s="4" t="s">
-        <v>198</v>
-      </c>
+      <c r="F133" s="4"/>
       <c r="G133" s="4"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -5443,13 +4881,13 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -5458,13 +4896,13 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -5472,35 +4910,29 @@
       <c r="G136" s="4"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C137" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E137" s="14" t="s">
-        <v>200</v>
-      </c>
+      <c r="A137" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
       <c r="F137" s="4"/>
-      <c r="G137" s="4">
-        <v>7</v>
-      </c>
+      <c r="G137" s="4"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>201</v>
+      <c r="A138" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -5509,13 +4941,13 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>202</v>
+        <v>32</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -5523,14 +4955,14 @@
       <c r="G139" s="4"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="s">
-        <v>203</v>
+      <c r="A140" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -5538,14 +4970,14 @@
       <c r="G140" s="4"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>36</v>
+      <c r="A141" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -5553,44 +4985,52 @@
       <c r="G141" s="4"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C142" s="1" t="s">
+      <c r="A142" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
       <c r="F142" s="4"/>
-      <c r="G142" s="4"/>
+      <c r="G142" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
-      <c r="F143" s="4"/>
+      <c r="F143" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="G143" s="4"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>38</v>
+        <v>199</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -5598,71 +5038,65 @@
       <c r="G144" s="4"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A145" s="14" t="s">
+      <c r="A145" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E147" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C145" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D145" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="E145" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F145" s="4"/>
-      <c r="G145" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C146" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E146" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="F146" s="4"/>
-      <c r="G146" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D147" s="4"/>
-      <c r="E147" s="4"/>
       <c r="F147" s="4"/>
-      <c r="G147" s="4"/>
+      <c r="G147" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
-        <v>41</v>
+      <c r="A148" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -5670,35 +5104,29 @@
       <c r="G148" s="4"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C149" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D149" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="E149" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="A149" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
       <c r="F149" s="4"/>
-      <c r="G149" s="4">
-        <v>1</v>
-      </c>
+      <c r="G149" s="4"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C150" s="10" t="s">
-        <v>153</v>
+        <v>203</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -5707,30 +5135,28 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
       <c r="F151" s="4"/>
-      <c r="G151" s="4">
-        <v>120</v>
-      </c>
+      <c r="G151" s="4"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="16" t="s">
-        <v>43</v>
+      <c r="A152" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -5738,14 +5164,14 @@
       <c r="G152" s="4"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="16" t="s">
-        <v>44</v>
+      <c r="A153" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -5753,14 +5179,14 @@
       <c r="G153" s="4"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A154" s="16" t="s">
-        <v>45</v>
+      <c r="A154" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -5768,46 +5194,56 @@
       <c r="G154" s="4"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D155" s="4"/>
-      <c r="E155" s="4"/>
+      <c r="A155" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D155" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E155" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="F155" s="4"/>
-      <c r="G155" s="4"/>
+      <c r="G155" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D156" s="4"/>
-      <c r="E156" s="4"/>
-      <c r="F156" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G156" s="4"/>
+      <c r="A156" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D156" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E156" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -5816,13 +5252,13 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -5830,19 +5266,25 @@
       <c r="G158" s="4"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A159" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D159" s="4"/>
-      <c r="E159" s="4"/>
+      <c r="A159" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D159" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E159" s="15" t="s">
+        <v>50</v>
+      </c>
       <c r="F159" s="4"/>
-      <c r="G159" s="4"/>
+      <c r="G159" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
@@ -6065,317 +5507,323 @@
       <c r="F172" s="4"/>
       <c r="G172" s="4"/>
     </row>
-    <row r="177" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="178" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="179" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="180" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="181" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="182" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="183" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="184" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="185" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="186" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="187" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <autoFilter ref="A1:G172" xr:uid="{F728FE19-0465-1C4B-A5E0-C11743CC7188}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="149" priority="115"/>
-    <cfRule type="duplicateValues" dxfId="148" priority="116"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="147"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="148"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="147" priority="117"/>
-    <cfRule type="duplicateValues" dxfId="146" priority="118"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="145" priority="101"/>
-    <cfRule type="duplicateValues" dxfId="144" priority="102"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A85">
-    <cfRule type="duplicateValues" dxfId="143" priority="97"/>
-    <cfRule type="duplicateValues" dxfId="142" priority="98"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A86 A3:A4 A34:A35 A51:A52 A67">
-    <cfRule type="duplicateValues" dxfId="141" priority="119"/>
-    <cfRule type="duplicateValues" dxfId="140" priority="120"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A87">
-    <cfRule type="duplicateValues" dxfId="139" priority="79"/>
-    <cfRule type="duplicateValues" dxfId="138" priority="80"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A101 A104 A106 A108 A110">
-    <cfRule type="duplicateValues" dxfId="137" priority="95"/>
-    <cfRule type="duplicateValues" dxfId="136" priority="96"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A145">
-    <cfRule type="duplicateValues" dxfId="135" priority="73"/>
-    <cfRule type="duplicateValues" dxfId="134" priority="74"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A149">
-    <cfRule type="duplicateValues" dxfId="133" priority="59"/>
-    <cfRule type="duplicateValues" dxfId="132" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="149"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="150"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:A42">
+    <cfRule type="duplicateValues" dxfId="153" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="78"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
+    <cfRule type="duplicateValues" dxfId="151" priority="133"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="134"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:A49">
+    <cfRule type="duplicateValues" dxfId="149" priority="163"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="164"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:A60">
+    <cfRule type="duplicateValues" dxfId="147" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="76"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:A75">
+    <cfRule type="duplicateValues" dxfId="145" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="74"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A76">
+    <cfRule type="duplicateValues" dxfId="143" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78">
+    <cfRule type="duplicateValues" dxfId="141" priority="169"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="170"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A79:A94">
+    <cfRule type="duplicateValues" dxfId="139" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="72"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A95">
+    <cfRule type="duplicateValues" dxfId="137" priority="129"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="130"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96 A13:A14 A44:A45 A77 A61">
+    <cfRule type="duplicateValues" dxfId="135" priority="151"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="152"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97">
+    <cfRule type="duplicateValues" dxfId="133" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="112"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98:A104">
+    <cfRule type="duplicateValues" dxfId="131" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="70"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A105">
+    <cfRule type="duplicateValues" dxfId="129" priority="175"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="176"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106:A109">
+    <cfRule type="duplicateValues" dxfId="127" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="68"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A110:A111 A114 A116 A118 A120">
+    <cfRule type="duplicateValues" dxfId="125" priority="127"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="128"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A112:A113">
+    <cfRule type="duplicateValues" dxfId="123" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="66"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115">
+    <cfRule type="duplicateValues" dxfId="121" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A117">
+    <cfRule type="duplicateValues" dxfId="119" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="62"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A119">
+    <cfRule type="duplicateValues" dxfId="117" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="60"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A121">
+    <cfRule type="duplicateValues" dxfId="115" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A124:A126">
+    <cfRule type="duplicateValues" dxfId="113" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A128:A130">
+    <cfRule type="duplicateValues" dxfId="111" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="54"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A136:A140 A132:A134">
+    <cfRule type="duplicateValues" dxfId="109" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A141">
+    <cfRule type="duplicateValues" dxfId="107" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="80"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A142">
+    <cfRule type="duplicateValues" dxfId="105" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="82"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A143:A146">
+    <cfRule type="duplicateValues" dxfId="103" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A148:A154">
+    <cfRule type="duplicateValues" dxfId="101" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A155">
+    <cfRule type="duplicateValues" dxfId="99" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="106"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A157:A158">
+    <cfRule type="duplicateValues" dxfId="97" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A159">
+    <cfRule type="duplicateValues" dxfId="95" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="92"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A162:A165">
+    <cfRule type="duplicateValues" dxfId="93" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A166">
-    <cfRule type="duplicateValues" dxfId="131" priority="63"/>
-    <cfRule type="duplicateValues" dxfId="130" priority="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A171 A112:A113 A137 A146 A150:A151 A117 A121 A160:A161">
-    <cfRule type="duplicateValues" dxfId="129" priority="121"/>
-    <cfRule type="duplicateValues" dxfId="128" priority="122"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="duplicateValues" dxfId="127" priority="99"/>
-    <cfRule type="duplicateValues" dxfId="126" priority="100"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="125" priority="111"/>
-    <cfRule type="duplicateValues" dxfId="124" priority="112"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D101">
-    <cfRule type="duplicateValues" dxfId="123" priority="93"/>
-    <cfRule type="duplicateValues" dxfId="122" priority="94"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104">
-    <cfRule type="duplicateValues" dxfId="121" priority="89"/>
-    <cfRule type="duplicateValues" dxfId="120" priority="90"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D106">
-    <cfRule type="duplicateValues" dxfId="119" priority="87"/>
-    <cfRule type="duplicateValues" dxfId="118" priority="88"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D108">
-    <cfRule type="duplicateValues" dxfId="117" priority="85"/>
-    <cfRule type="duplicateValues" dxfId="116" priority="86"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D132">
-    <cfRule type="duplicateValues" dxfId="115" priority="103"/>
-    <cfRule type="duplicateValues" dxfId="114" priority="104"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D137">
-    <cfRule type="duplicateValues" dxfId="113" priority="109"/>
-    <cfRule type="duplicateValues" dxfId="112" priority="110"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D145">
-    <cfRule type="duplicateValues" dxfId="111" priority="71"/>
-    <cfRule type="duplicateValues" dxfId="110" priority="72"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D146">
-    <cfRule type="duplicateValues" dxfId="109" priority="107"/>
-    <cfRule type="duplicateValues" dxfId="108" priority="108"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D149">
-    <cfRule type="duplicateValues" dxfId="107" priority="77"/>
-    <cfRule type="duplicateValues" dxfId="106" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="96"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A168:A169">
+    <cfRule type="duplicateValues" dxfId="89" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A171 A122:A123 A147 A156 A127 A131 A160:A161">
+    <cfRule type="duplicateValues" dxfId="87" priority="153"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="154"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A172">
+    <cfRule type="duplicateValues" dxfId="85" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C117">
+    <cfRule type="duplicateValues" dxfId="83" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C119">
+    <cfRule type="duplicateValues" dxfId="81" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="duplicateValues" dxfId="79" priority="155"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="156"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="duplicateValues" dxfId="77" priority="159"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="160"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="duplicateValues" dxfId="75" priority="165"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="166"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D76">
+    <cfRule type="duplicateValues" dxfId="73" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="duplicateValues" dxfId="71" priority="173"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="174"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D95">
+    <cfRule type="duplicateValues" dxfId="69" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="86"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D97">
+    <cfRule type="duplicateValues" dxfId="67" priority="143"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="144"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D105">
+    <cfRule type="duplicateValues" dxfId="65" priority="177"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="178"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D111">
+    <cfRule type="duplicateValues" dxfId="63" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="126"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D114">
+    <cfRule type="duplicateValues" dxfId="61" priority="121"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="122"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D116">
+    <cfRule type="duplicateValues" dxfId="59" priority="119"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="120"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D118">
+    <cfRule type="duplicateValues" dxfId="57" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="118"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D131">
+    <cfRule type="duplicateValues" dxfId="55" priority="179"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="180"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D142">
+    <cfRule type="duplicateValues" dxfId="53" priority="135"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="136"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D147">
+    <cfRule type="duplicateValues" dxfId="51" priority="141"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="142"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D155">
+    <cfRule type="duplicateValues" dxfId="49" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="104"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D156">
+    <cfRule type="duplicateValues" dxfId="47" priority="139"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="140"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D159">
+    <cfRule type="duplicateValues" dxfId="45" priority="109"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="duplicateValues" dxfId="105" priority="65"/>
-    <cfRule type="duplicateValues" dxfId="104" priority="66"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="duplicateValues" dxfId="103" priority="113"/>
-    <cfRule type="duplicateValues" dxfId="102" priority="114"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E101">
-    <cfRule type="duplicateValues" dxfId="101" priority="91"/>
-    <cfRule type="duplicateValues" dxfId="100" priority="92"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E104">
-    <cfRule type="duplicateValues" dxfId="99" priority="83"/>
-    <cfRule type="duplicateValues" dxfId="98" priority="84"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
-    <cfRule type="duplicateValues" dxfId="97" priority="81"/>
-    <cfRule type="duplicateValues" dxfId="96" priority="82"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E132">
-    <cfRule type="duplicateValues" dxfId="95" priority="105"/>
-    <cfRule type="duplicateValues" dxfId="94" priority="106"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E137">
-    <cfRule type="duplicateValues" dxfId="93" priority="67"/>
-    <cfRule type="duplicateValues" dxfId="92" priority="68"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E145">
-    <cfRule type="duplicateValues" dxfId="91" priority="69"/>
-    <cfRule type="duplicateValues" dxfId="90" priority="70"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
-    <cfRule type="duplicateValues" dxfId="89" priority="75"/>
-    <cfRule type="duplicateValues" dxfId="88" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="98"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="duplicateValues" dxfId="41" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="duplicateValues" dxfId="39" priority="161"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="162"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule type="duplicateValues" dxfId="37" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E76">
+    <cfRule type="duplicateValues" dxfId="35" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E78">
+    <cfRule type="duplicateValues" dxfId="33" priority="171"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="172"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95">
+    <cfRule type="duplicateValues" dxfId="31" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="84"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E111">
+    <cfRule type="duplicateValues" dxfId="29" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="124"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E114">
+    <cfRule type="duplicateValues" dxfId="27" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="116"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E116">
+    <cfRule type="duplicateValues" dxfId="25" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="114"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E127">
+    <cfRule type="duplicateValues" dxfId="23" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E131">
+    <cfRule type="duplicateValues" dxfId="21" priority="181"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="182"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E142">
+    <cfRule type="duplicateValues" dxfId="19" priority="137"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="138"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E147">
+    <cfRule type="duplicateValues" dxfId="17" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="100"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E155">
+    <cfRule type="duplicateValues" dxfId="15" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="102"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E156">
+    <cfRule type="duplicateValues" dxfId="13" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="90"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E159">
+    <cfRule type="duplicateValues" dxfId="11" priority="107"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E161">
-    <cfRule type="duplicateValues" dxfId="87" priority="61"/>
-    <cfRule type="duplicateValues" dxfId="86" priority="62"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E146">
-    <cfRule type="duplicateValues" dxfId="85" priority="57"/>
-    <cfRule type="duplicateValues" dxfId="84" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E170">
-    <cfRule type="duplicateValues" dxfId="83" priority="55"/>
-    <cfRule type="duplicateValues" dxfId="82" priority="56"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
-    <cfRule type="duplicateValues" dxfId="81" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="54"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
-    <cfRule type="duplicateValues" dxfId="79" priority="51"/>
-    <cfRule type="duplicateValues" dxfId="78" priority="52"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A132">
-    <cfRule type="duplicateValues" dxfId="77" priority="49"/>
-    <cfRule type="duplicateValues" dxfId="76" priority="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A131">
-    <cfRule type="duplicateValues" dxfId="75" priority="47"/>
-    <cfRule type="duplicateValues" dxfId="74" priority="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A32">
-    <cfRule type="duplicateValues" dxfId="73" priority="45"/>
-    <cfRule type="duplicateValues" dxfId="72" priority="46"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="71" priority="123"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="124"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="69" priority="125"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="126"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="duplicateValues" dxfId="67" priority="127"/>
-    <cfRule type="duplicateValues" dxfId="66" priority="128"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="duplicateValues" dxfId="65" priority="129"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="130"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40:A50">
-    <cfRule type="duplicateValues" dxfId="63" priority="43"/>
-    <cfRule type="duplicateValues" dxfId="62" priority="44"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36:A39">
-    <cfRule type="duplicateValues" dxfId="61" priority="131"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="132"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53:A66">
-    <cfRule type="duplicateValues" dxfId="59" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="42"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="duplicateValues" dxfId="57" priority="133"/>
-    <cfRule type="duplicateValues" dxfId="56" priority="134"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="duplicateValues" dxfId="55" priority="135"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="136"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69:A84">
-    <cfRule type="duplicateValues" dxfId="53" priority="39"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68">
-    <cfRule type="duplicateValues" dxfId="51" priority="137"/>
-    <cfRule type="duplicateValues" dxfId="50" priority="138"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="duplicateValues" dxfId="49" priority="139"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="140"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="duplicateValues" dxfId="47" priority="141"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="142"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A88:A94">
-    <cfRule type="duplicateValues" dxfId="45" priority="37"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96:A99">
-    <cfRule type="duplicateValues" dxfId="43" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="42" priority="36"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A95">
-    <cfRule type="duplicateValues" dxfId="41" priority="143"/>
-    <cfRule type="duplicateValues" dxfId="40" priority="144"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D95">
-    <cfRule type="duplicateValues" dxfId="39" priority="145"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="146"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A102:A103">
-    <cfRule type="duplicateValues" dxfId="37" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
-    <cfRule type="duplicateValues" dxfId="35" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
-    <cfRule type="duplicateValues" dxfId="33" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A109">
-    <cfRule type="duplicateValues" dxfId="31" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A111">
-    <cfRule type="duplicateValues" dxfId="29" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A114:A116">
-    <cfRule type="duplicateValues" dxfId="27" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A118:A120">
-    <cfRule type="duplicateValues" dxfId="25" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A126:A130 A122:A124">
-    <cfRule type="duplicateValues" dxfId="23" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D121">
-    <cfRule type="duplicateValues" dxfId="21" priority="147"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="148"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E121">
-    <cfRule type="duplicateValues" dxfId="19" priority="149"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="150"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A133:A136">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A138:A144">
-    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A147:A148">
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A152:A159">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A162:A165">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A168:A169">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A172">
+    <cfRule type="duplicateValues" dxfId="7" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="88"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D127">
     <cfRule type="duplicateValues" dxfId="5" priority="5"/>
     <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C109">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="A5:A12">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A4">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update pilot template file
</commit_message>
<xml_diff>
--- a/templates/IssueBluePrintPilot.xlsx
+++ b/templates/IssueBluePrintPilot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephankuche/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephankuche/CreateJiraIssues/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E364D9FE-EB42-7448-ADB2-89D4B2581374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C7DBCD-D421-3D43-B7A0-44FB5B39D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="500" windowWidth="40040" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
@@ -3003,10 +3003,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD5E05C-EBFE-384E-9214-D4F9000DB306}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D219" sqref="D219"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3041,7 +3042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>138</v>
       </c>
@@ -3053,7 +3054,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>37</v>
       </c>
@@ -3104,7 +3105,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
@@ -3119,7 +3120,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>39</v>
       </c>
@@ -3134,7 +3135,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -3149,7 +3150,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -3166,7 +3167,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>230</v>
       </c>
@@ -3181,7 +3182,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -3196,7 +3197,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -3211,7 +3212,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
@@ -3239,9 +3240,11 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>139</v>
       </c>
@@ -3294,7 +3297,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>141</v>
       </c>
@@ -3311,7 +3314,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -3328,7 +3331,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -3343,7 +3346,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -3360,7 +3363,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
@@ -3375,7 +3378,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>142</v>
       </c>
@@ -3392,7 +3395,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
@@ -3409,7 +3412,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
@@ -3424,7 +3427,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -3441,7 +3444,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>193</v>
       </c>
@@ -3456,7 +3459,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
@@ -3471,7 +3474,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
@@ -3486,7 +3489,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -3501,7 +3504,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
@@ -3518,7 +3521,7 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -3533,7 +3536,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>75</v>
       </c>
@@ -3550,7 +3553,7 @@
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
@@ -3565,7 +3568,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
@@ -3580,7 +3583,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>79</v>
       </c>
@@ -3595,7 +3598,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>80</v>
       </c>
@@ -3612,7 +3615,7 @@
       </c>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>81</v>
       </c>
@@ -3629,7 +3632,7 @@
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>82</v>
       </c>
@@ -3646,7 +3649,7 @@
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>143</v>
       </c>
@@ -3663,7 +3666,7 @@
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>145</v>
       </c>
@@ -3680,7 +3683,7 @@
       </c>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -3695,7 +3698,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -3710,7 +3713,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -3742,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>88</v>
       </c>
@@ -3789,7 +3792,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>245</v>
       </c>
@@ -3804,7 +3807,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>89</v>
       </c>
@@ -3821,7 +3824,7 @@
       </c>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>90</v>
       </c>
@@ -3836,7 +3839,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>91</v>
       </c>
@@ -3851,7 +3854,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>92</v>
       </c>
@@ -3868,7 +3871,7 @@
       </c>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>94</v>
       </c>
@@ -3883,7 +3886,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -3900,7 +3903,7 @@
       </c>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
@@ -3915,7 +3918,7 @@
       <c r="F56" s="2"/>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>98</v>
       </c>
@@ -3932,7 +3935,7 @@
       </c>
       <c r="G57" s="4"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
@@ -3947,7 +3950,7 @@
       <c r="F58" s="2"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>101</v>
       </c>
@@ -3962,7 +3965,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>192</v>
       </c>
@@ -3977,7 +3980,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>190</v>
       </c>
@@ -3992,7 +3995,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>244</v>
       </c>
@@ -4007,7 +4010,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>191</v>
       </c>
@@ -4022,7 +4025,7 @@
       <c r="F63" s="2"/>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>246</v>
       </c>
@@ -4037,7 +4040,7 @@
       <c r="F64" s="2"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>217</v>
       </c>
@@ -4052,7 +4055,7 @@
       <c r="F65" s="2"/>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>247</v>
       </c>
@@ -4067,7 +4070,7 @@
       <c r="F66" s="2"/>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>249</v>
       </c>
@@ -4082,7 +4085,7 @@
       <c r="F67" s="2"/>
       <c r="G67" s="4"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>250</v>
       </c>
@@ -4097,7 +4100,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>184</v>
       </c>
@@ -4112,7 +4115,7 @@
       <c r="F69" s="2"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>183</v>
       </c>
@@ -4127,7 +4130,7 @@
       <c r="F70" s="2"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>186</v>
       </c>
@@ -4142,7 +4145,7 @@
       <c r="F71" s="2"/>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>188</v>
       </c>
@@ -4157,7 +4160,7 @@
       <c r="F72" s="2"/>
       <c r="G72" s="4"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>189</v>
       </c>
@@ -4172,7 +4175,7 @@
       <c r="F73" s="2"/>
       <c r="G73" s="4"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>187</v>
       </c>
@@ -4187,7 +4190,7 @@
       <c r="F74" s="2"/>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>182</v>
       </c>
@@ -4202,7 +4205,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="4"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>185</v>
       </c>
@@ -4217,7 +4220,7 @@
       <c r="F76" s="2"/>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>251</v>
       </c>
@@ -4232,7 +4235,7 @@
       <c r="F77" s="2"/>
       <c r="G77" s="4"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>252</v>
       </c>
@@ -4247,7 +4250,7 @@
       <c r="F78" s="2"/>
       <c r="G78" s="4"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>102</v>
       </c>
@@ -4262,7 +4265,7 @@
       <c r="F79" s="2"/>
       <c r="G79" s="4"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>254</v>
       </c>
@@ -4300,7 +4303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>103</v>
       </c>
@@ -4317,7 +4320,7 @@
       </c>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>104</v>
       </c>
@@ -4334,7 +4337,7 @@
       </c>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>106</v>
       </c>
@@ -4351,7 +4354,7 @@
       </c>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>150</v>
       </c>
@@ -4368,7 +4371,7 @@
       </c>
       <c r="G85" s="4"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>109</v>
       </c>
@@ -4385,7 +4388,7 @@
       </c>
       <c r="G86" s="4"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>111</v>
       </c>
@@ -4402,7 +4405,7 @@
       </c>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>112</v>
       </c>
@@ -4419,7 +4422,7 @@
       </c>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>114</v>
       </c>
@@ -4436,7 +4439,7 @@
       </c>
       <c r="G89" s="4"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>115</v>
       </c>
@@ -4451,7 +4454,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>116</v>
       </c>
@@ -4468,7 +4471,7 @@
       </c>
       <c r="G91" s="4"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>154</v>
       </c>
@@ -4485,7 +4488,7 @@
       </c>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>156</v>
       </c>
@@ -4502,7 +4505,7 @@
       </c>
       <c r="G93" s="4"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>117</v>
       </c>
@@ -4517,7 +4520,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>118</v>
       </c>
@@ -4553,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>119</v>
       </c>
@@ -4589,7 +4592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>120</v>
       </c>
@@ -4604,7 +4607,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>121</v>
       </c>
@@ -4619,7 +4622,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>122</v>
       </c>
@@ -4634,7 +4637,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>123</v>
       </c>
@@ -4649,7 +4652,7 @@
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>124</v>
       </c>
@@ -4664,7 +4667,7 @@
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>125</v>
       </c>
@@ -4681,7 +4684,7 @@
       </c>
       <c r="G104" s="4"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>126</v>
       </c>
@@ -4696,7 +4699,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>158</v>
       </c>
@@ -4711,7 +4714,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>159</v>
       </c>
@@ -4726,7 +4729,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>127</v>
       </c>
@@ -4741,7 +4744,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>128</v>
       </c>
@@ -4756,7 +4759,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>129</v>
       </c>
@@ -4771,7 +4774,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>160</v>
       </c>
@@ -4786,7 +4789,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>130</v>
       </c>
@@ -4801,7 +4804,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>231</v>
       </c>
@@ -4816,7 +4819,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>232</v>
       </c>
@@ -4852,7 +4855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>10</v>
       </c>
@@ -4884,7 +4887,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>242</v>
       </c>
@@ -4916,7 +4919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>248</v>
       </c>
@@ -4931,7 +4934,7 @@
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>255</v>
       </c>
@@ -4946,7 +4949,7 @@
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>243</v>
       </c>
@@ -4961,7 +4964,7 @@
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>11</v>
       </c>
@@ -4976,7 +4979,7 @@
       <c r="F123" s="4"/>
       <c r="G123" s="4"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>12</v>
       </c>
@@ -4991,7 +4994,7 @@
       <c r="F124" s="4"/>
       <c r="G124" s="4"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>13</v>
       </c>
@@ -5006,7 +5009,7 @@
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>195</v>
       </c>
@@ -5034,9 +5037,11 @@
       <c r="D127" s="17"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
-      <c r="G127" s="4"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G127" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>198</v>
       </c>
@@ -5051,7 +5056,7 @@
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>199</v>
       </c>
@@ -5066,7 +5071,7 @@
       <c r="F129" s="4"/>
       <c r="G129" s="4"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>200</v>
       </c>
@@ -5081,7 +5086,7 @@
       <c r="F130" s="4"/>
       <c r="G130" s="4"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>197</v>
       </c>
@@ -5109,9 +5114,11 @@
       <c r="D132" s="17"/>
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G132" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>202</v>
       </c>
@@ -5126,7 +5133,7 @@
       <c r="F133" s="4"/>
       <c r="G133" s="4"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>205</v>
       </c>
@@ -5141,7 +5148,7 @@
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>203</v>
       </c>
@@ -5156,7 +5163,7 @@
       <c r="F135" s="4"/>
       <c r="G135" s="4"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>204</v>
       </c>
@@ -5184,9 +5191,11 @@
       <c r="D137" s="17"/>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
-      <c r="G137" s="4"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G137" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>207</v>
       </c>
@@ -5201,7 +5210,7 @@
       <c r="F138" s="4"/>
       <c r="G138" s="4"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>214</v>
       </c>
@@ -5216,7 +5225,7 @@
       <c r="F139" s="4"/>
       <c r="G139" s="4"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>208</v>
       </c>
@@ -5231,7 +5240,7 @@
       <c r="F140" s="4"/>
       <c r="G140" s="4"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>209</v>
       </c>
@@ -5259,9 +5268,11 @@
       <c r="D142" s="17"/>
       <c r="E142" s="4"/>
       <c r="F142" s="4"/>
-      <c r="G142" s="4"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G142" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>212</v>
       </c>
@@ -5276,7 +5287,7 @@
       <c r="F143" s="4"/>
       <c r="G143" s="4"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>215</v>
       </c>
@@ -5291,7 +5302,7 @@
       <c r="F144" s="4"/>
       <c r="G144" s="4"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>211</v>
       </c>
@@ -5306,7 +5317,7 @@
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>213</v>
       </c>
@@ -5334,9 +5345,11 @@
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
-      <c r="G147" s="4"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G147" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>223</v>
       </c>
@@ -5364,9 +5377,11 @@
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
-      <c r="G149" s="4"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G149" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>224</v>
       </c>
@@ -5394,9 +5409,11 @@
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
       <c r="F151" s="4"/>
-      <c r="G151" s="4"/>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G151" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>226</v>
       </c>
@@ -5411,7 +5428,7 @@
       <c r="F152" s="4"/>
       <c r="G152" s="4"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>225</v>
       </c>
@@ -5426,7 +5443,7 @@
       <c r="F153" s="4"/>
       <c r="G153" s="4"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>14</v>
       </c>
@@ -5458,7 +5475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>52</v>
       </c>
@@ -5473,7 +5490,7 @@
       <c r="F156" s="4"/>
       <c r="G156" s="4"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>16</v>
       </c>
@@ -5505,7 +5522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>17</v>
       </c>
@@ -5537,7 +5554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>19</v>
       </c>
@@ -5569,7 +5586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>18</v>
       </c>
@@ -5601,7 +5618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>20</v>
       </c>
@@ -5686,7 +5703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>21</v>
       </c>
@@ -5718,7 +5735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>166</v>
       </c>
@@ -5735,7 +5752,7 @@
       </c>
       <c r="G172" s="4"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>167</v>
       </c>
@@ -5752,7 +5769,7 @@
       </c>
       <c r="G173" s="4"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>168</v>
       </c>
@@ -5790,7 +5807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>23</v>
       </c>
@@ -5805,7 +5822,7 @@
       <c r="F176" s="4"/>
       <c r="G176" s="4"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>228</v>
       </c>
@@ -5820,7 +5837,7 @@
       <c r="F177" s="4"/>
       <c r="G177" s="4"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="13" t="s">
         <v>29</v>
       </c>
@@ -5835,7 +5852,7 @@
       <c r="F178" s="4"/>
       <c r="G178" s="4"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>229</v>
       </c>
@@ -5850,7 +5867,7 @@
       <c r="F179" s="4"/>
       <c r="G179" s="4"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>238</v>
       </c>
@@ -5882,7 +5899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>222</v>
       </c>
@@ -5897,7 +5914,7 @@
       <c r="F182" s="4"/>
       <c r="G182" s="4"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>25</v>
       </c>
@@ -5912,7 +5929,7 @@
       <c r="F183" s="4"/>
       <c r="G183" s="4"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>26</v>
       </c>
@@ -5927,7 +5944,7 @@
       <c r="F184" s="4"/>
       <c r="G184" s="4"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>27</v>
       </c>
@@ -5942,7 +5959,7 @@
       <c r="F185" s="4"/>
       <c r="G185" s="4"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>28</v>
       </c>
@@ -5957,7 +5974,7 @@
       <c r="F186" s="4"/>
       <c r="G186" s="4"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="13" t="s">
         <v>169</v>
       </c>
@@ -5993,7 +6010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>170</v>
       </c>
@@ -6010,7 +6027,7 @@
       </c>
       <c r="G189" s="4"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>172</v>
       </c>
@@ -6025,7 +6042,7 @@
       <c r="F190" s="4"/>
       <c r="G190" s="4"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>133</v>
       </c>
@@ -6040,7 +6057,7 @@
       <c r="F191" s="4"/>
       <c r="G191" s="4"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>135</v>
       </c>
@@ -6076,7 +6093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>173</v>
       </c>
@@ -6091,7 +6108,7 @@
       <c r="F194" s="4"/>
       <c r="G194" s="4"/>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>174</v>
       </c>
@@ -6106,7 +6123,7 @@
       <c r="F195" s="4"/>
       <c r="G195" s="4"/>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>175</v>
       </c>
@@ -6121,7 +6138,7 @@
       <c r="F196" s="4"/>
       <c r="G196" s="4"/>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>31</v>
       </c>
@@ -6136,7 +6153,7 @@
       <c r="F197" s="4"/>
       <c r="G197" s="4"/>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>176</v>
       </c>
@@ -6151,7 +6168,7 @@
       <c r="F198" s="4"/>
       <c r="G198" s="4"/>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>177</v>
       </c>
@@ -6166,7 +6183,7 @@
       <c r="F199" s="4"/>
       <c r="G199" s="4"/>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>32</v>
       </c>
@@ -6223,7 +6240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>34</v>
       </c>
@@ -6238,7 +6255,7 @@
       <c r="F203" s="4"/>
       <c r="G203" s="4"/>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>35</v>
       </c>
@@ -6253,7 +6270,7 @@
       <c r="F204" s="4"/>
       <c r="G204" s="4"/>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>258</v>
       </c>
@@ -6268,7 +6285,7 @@
       <c r="F205" s="4"/>
       <c r="G205" s="4"/>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>257</v>
       </c>
@@ -6304,7 +6321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>43</v>
       </c>
@@ -6340,7 +6357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>45</v>
       </c>
@@ -6355,7 +6372,7 @@
       <c r="F210" s="4"/>
       <c r="G210" s="4"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="15" t="s">
         <v>46</v>
       </c>
@@ -6370,7 +6387,7 @@
       <c r="F211" s="4"/>
       <c r="G211" s="4"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="15" t="s">
         <v>47</v>
       </c>
@@ -6385,7 +6402,7 @@
       <c r="F212" s="4"/>
       <c r="G212" s="4"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>53</v>
       </c>
@@ -6400,7 +6417,7 @@
       <c r="F213" s="4"/>
       <c r="G213" s="4"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="15" t="s">
         <v>48</v>
       </c>
@@ -6457,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>259</v>
       </c>
@@ -6472,7 +6489,7 @@
       <c r="F217" s="4"/>
       <c r="G217" s="4"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>49</v>
       </c>
@@ -6525,7 +6542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>51</v>
       </c>
@@ -6541,18 +6558,24 @@
       <c r="G221" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G221" xr:uid="{F728FE19-0465-1C4B-A5E0-C11743CC7188}"/>
+  <autoFilter ref="A1:G221" xr:uid="{F728FE19-0465-1C4B-A5E0-C11743CC7188}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Task"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="169" priority="223"/>
-    <cfRule type="duplicateValues" dxfId="168" priority="224"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="224"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="223"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="167" priority="225"/>
     <cfRule type="duplicateValues" dxfId="166" priority="226"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4">
-    <cfRule type="duplicateValues" dxfId="165" priority="79"/>
-    <cfRule type="duplicateValues" dxfId="164" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A14">
     <cfRule type="duplicateValues" dxfId="163" priority="77"/>
@@ -6563,324 +6586,324 @@
     <cfRule type="duplicateValues" dxfId="160" priority="260"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="duplicateValues" dxfId="159" priority="209"/>
-    <cfRule type="duplicateValues" dxfId="158" priority="210"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="210"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="209"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:A52">
-    <cfRule type="duplicateValues" dxfId="157" priority="239"/>
-    <cfRule type="duplicateValues" dxfId="156" priority="240"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="240"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="239"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53:A80">
+    <cfRule type="duplicateValues" dxfId="155" priority="416"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="415"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:A95">
-    <cfRule type="duplicateValues" dxfId="155" priority="149"/>
-    <cfRule type="duplicateValues" dxfId="154" priority="150"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="150"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="149"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="duplicateValues" dxfId="153" priority="95"/>
-    <cfRule type="duplicateValues" dxfId="152" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="duplicateValues" dxfId="151" priority="245"/>
-    <cfRule type="duplicateValues" dxfId="150" priority="246"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="246"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="245"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:A114">
-    <cfRule type="duplicateValues" dxfId="149" priority="147"/>
-    <cfRule type="duplicateValues" dxfId="148" priority="148"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="148"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="147"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="duplicateValues" dxfId="147" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="146" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116 A15:A16 A46:A47 A97 A81">
-    <cfRule type="duplicateValues" dxfId="145" priority="227"/>
-    <cfRule type="duplicateValues" dxfId="144" priority="228"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="227"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="228"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A117 A119">
-    <cfRule type="duplicateValues" dxfId="143" priority="187"/>
-    <cfRule type="duplicateValues" dxfId="142" priority="188"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="187"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="188"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118">
-    <cfRule type="duplicateValues" dxfId="141" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="140" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A120:A126">
+    <cfRule type="duplicateValues" dxfId="137" priority="420"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="419"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A148">
-    <cfRule type="duplicateValues" dxfId="139" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="138" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150">
-    <cfRule type="duplicateValues" dxfId="137" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="136" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151 A127:A147 A149">
-    <cfRule type="duplicateValues" dxfId="135" priority="331"/>
-    <cfRule type="duplicateValues" dxfId="134" priority="332"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="332"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="331"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="133" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="132" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154:A155 A158 A160 A162 A164">
-    <cfRule type="duplicateValues" dxfId="131" priority="203"/>
-    <cfRule type="duplicateValues" dxfId="130" priority="204"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="203"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="204"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:A157">
-    <cfRule type="duplicateValues" dxfId="129" priority="141"/>
-    <cfRule type="duplicateValues" dxfId="128" priority="142"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="142"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="141"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A159">
-    <cfRule type="duplicateValues" dxfId="127" priority="139"/>
-    <cfRule type="duplicateValues" dxfId="126" priority="140"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="140"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="139"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A161">
-    <cfRule type="duplicateValues" dxfId="125" priority="137"/>
-    <cfRule type="duplicateValues" dxfId="124" priority="138"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="137"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="138"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A163">
-    <cfRule type="duplicateValues" dxfId="123" priority="135"/>
-    <cfRule type="duplicateValues" dxfId="122" priority="136"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="135"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="136"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A165">
-    <cfRule type="duplicateValues" dxfId="121" priority="133"/>
-    <cfRule type="duplicateValues" dxfId="120" priority="134"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="133"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="134"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A168:A169">
-    <cfRule type="duplicateValues" dxfId="119" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="118" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172:A174">
-    <cfRule type="duplicateValues" dxfId="117" priority="131"/>
-    <cfRule type="duplicateValues" dxfId="116" priority="132"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="132"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="131"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A176:A177 A179:A180">
-    <cfRule type="duplicateValues" dxfId="115" priority="347"/>
-    <cfRule type="duplicateValues" dxfId="114" priority="348"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="348"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="347"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A178">
-    <cfRule type="duplicateValues" dxfId="113" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="112" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182:A186">
-    <cfRule type="duplicateValues" dxfId="111" priority="333"/>
-    <cfRule type="duplicateValues" dxfId="110" priority="334"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="333"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="334"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A187">
-    <cfRule type="duplicateValues" dxfId="109" priority="155"/>
-    <cfRule type="duplicateValues" dxfId="108" priority="156"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="155"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="156"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A188">
-    <cfRule type="duplicateValues" dxfId="107" priority="157"/>
-    <cfRule type="duplicateValues" dxfId="106" priority="158"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="157"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="158"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A189:A192">
-    <cfRule type="duplicateValues" dxfId="105" priority="125"/>
-    <cfRule type="duplicateValues" dxfId="104" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194:A200">
-    <cfRule type="duplicateValues" dxfId="103" priority="123"/>
-    <cfRule type="duplicateValues" dxfId="102" priority="124"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="124"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A201">
-    <cfRule type="duplicateValues" dxfId="101" priority="181"/>
-    <cfRule type="duplicateValues" dxfId="100" priority="182"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="181"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="182"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203:A206">
-    <cfRule type="duplicateValues" dxfId="99" priority="121"/>
-    <cfRule type="duplicateValues" dxfId="98" priority="122"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="122"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A207">
-    <cfRule type="duplicateValues" dxfId="97" priority="167"/>
-    <cfRule type="duplicateValues" dxfId="96" priority="168"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="167"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="168"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A213">
+    <cfRule type="duplicateValues" dxfId="91" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A214 A210:A212">
+    <cfRule type="duplicateValues" dxfId="89" priority="421"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="422"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A215">
-    <cfRule type="duplicateValues" dxfId="95" priority="171"/>
-    <cfRule type="duplicateValues" dxfId="94" priority="172"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="171"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="172"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A217:A218">
+    <cfRule type="duplicateValues" dxfId="85" priority="424"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="423"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A220 A170:A171 A193 A202 A175 A181 A208:A209">
-    <cfRule type="duplicateValues" dxfId="93" priority="229"/>
-    <cfRule type="duplicateValues" dxfId="92" priority="230"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="230"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="229"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A221">
-    <cfRule type="duplicateValues" dxfId="91" priority="113"/>
-    <cfRule type="duplicateValues" dxfId="90" priority="114"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118">
-    <cfRule type="duplicateValues" dxfId="89" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="88" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="87" priority="73"/>
-    <cfRule type="duplicateValues" dxfId="86" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="duplicateValues" dxfId="85" priority="231"/>
-    <cfRule type="duplicateValues" dxfId="84" priority="232"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="232"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="231"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="83" priority="235"/>
-    <cfRule type="duplicateValues" dxfId="82" priority="236"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="236"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="235"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="duplicateValues" dxfId="81" priority="241"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="242"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="242"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="241"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="duplicateValues" dxfId="79" priority="91"/>
-    <cfRule type="duplicateValues" dxfId="78" priority="92"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="duplicateValues" dxfId="77" priority="249"/>
-    <cfRule type="duplicateValues" dxfId="76" priority="250"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="250"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="249"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D115">
-    <cfRule type="duplicateValues" dxfId="75" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="74" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117 D119">
-    <cfRule type="duplicateValues" dxfId="73" priority="219"/>
-    <cfRule type="duplicateValues" dxfId="72" priority="220"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="220"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="219"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D155">
-    <cfRule type="duplicateValues" dxfId="71" priority="201"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="202"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="201"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="202"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D158">
-    <cfRule type="duplicateValues" dxfId="69" priority="197"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="198"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="197"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="198"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D160">
-    <cfRule type="duplicateValues" dxfId="67" priority="195"/>
-    <cfRule type="duplicateValues" dxfId="66" priority="196"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="195"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="196"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="duplicateValues" dxfId="65" priority="193"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="194"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="194"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="193"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175">
-    <cfRule type="duplicateValues" dxfId="63" priority="81"/>
-    <cfRule type="duplicateValues" dxfId="62" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D181">
-    <cfRule type="duplicateValues" dxfId="61" priority="255"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="256"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="256"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="255"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D188">
-    <cfRule type="duplicateValues" dxfId="59" priority="211"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="212"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="211"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="212"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D193">
-    <cfRule type="duplicateValues" dxfId="57" priority="217"/>
-    <cfRule type="duplicateValues" dxfId="56" priority="218"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="218"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="217"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D201">
-    <cfRule type="duplicateValues" dxfId="55" priority="179"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="180"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="180"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="179"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D202">
-    <cfRule type="duplicateValues" dxfId="53" priority="215"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="216"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="216"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="215"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D207">
-    <cfRule type="duplicateValues" dxfId="51" priority="185"/>
-    <cfRule type="duplicateValues" dxfId="50" priority="186"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="186"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="185"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D215">
-    <cfRule type="duplicateValues" dxfId="49" priority="173"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="174"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="173"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="174"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="47" priority="75"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="duplicateValues" dxfId="45" priority="107"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="duplicateValues" dxfId="43" priority="237"/>
-    <cfRule type="duplicateValues" dxfId="42" priority="238"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="237"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="238"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="duplicateValues" dxfId="41" priority="89"/>
-    <cfRule type="duplicateValues" dxfId="40" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="duplicateValues" dxfId="39" priority="87"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E98">
-    <cfRule type="duplicateValues" dxfId="37" priority="247"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="248"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="247"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="248"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E115">
-    <cfRule type="duplicateValues" dxfId="35" priority="159"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="160"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="159"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="160"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E155">
-    <cfRule type="duplicateValues" dxfId="33" priority="199"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="200"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="200"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="199"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158">
-    <cfRule type="duplicateValues" dxfId="31" priority="191"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="192"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="191"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="192"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E160">
-    <cfRule type="duplicateValues" dxfId="29" priority="189"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="190"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="189"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="190"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E175">
-    <cfRule type="duplicateValues" dxfId="27" priority="85"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E181">
-    <cfRule type="duplicateValues" dxfId="25" priority="257"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="258"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="258"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="257"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E188">
-    <cfRule type="duplicateValues" dxfId="23" priority="213"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="214"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="213"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E193">
-    <cfRule type="duplicateValues" dxfId="21" priority="175"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="176"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="175"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="176"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E201">
-    <cfRule type="duplicateValues" dxfId="19" priority="177"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="178"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="178"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="177"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E202">
-    <cfRule type="duplicateValues" dxfId="17" priority="165"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="166"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="166"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="165"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E207">
-    <cfRule type="duplicateValues" dxfId="15" priority="183"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="184"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="184"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="183"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E209">
-    <cfRule type="duplicateValues" dxfId="13" priority="169"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="170"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="169"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="170"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E219">
-    <cfRule type="duplicateValues" dxfId="11" priority="163"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="164"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53:A80">
-    <cfRule type="duplicateValues" dxfId="9" priority="415"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="416"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A120:A126">
-    <cfRule type="duplicateValues" dxfId="7" priority="419"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="420"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A214 A210:A212">
-    <cfRule type="duplicateValues" dxfId="5" priority="421"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="422"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A213">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A217:A218">
-    <cfRule type="duplicateValues" dxfId="1" priority="423"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="424"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="164"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="163"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the blueprintfiles poc & pilot
</commit_message>
<xml_diff>
--- a/templates/IssueBluePrintPilot.xlsx
+++ b/templates/IssueBluePrintPilot.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephankuche/CreateJiraIssues/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BCBFD3-3D84-8645-8261-A92887952B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AA5649-4BE8-0B42-AA56-1FE8AF4382BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18120" yWindow="500" windowWidth="33080" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="500" windowWidth="33080" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$220</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="259">
   <si>
     <t>Summary</t>
   </si>
@@ -786,9 +786,6 @@
   </si>
   <si>
     <t>Copy documents to in Context Learning Project</t>
-  </si>
-  <si>
-    <t>MileStone_SIT_approval</t>
   </si>
   <si>
     <t>Present Results Overview Slidedeck</t>
@@ -1004,57 +1001,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="181">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="176">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3113,10 +3060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD5E05C-EBFE-384E-9214-D4F9000DB306}">
-  <dimension ref="A1:G221"/>
+  <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175:E175"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3196,7 +3143,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3378,15 +3325,11 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4">
-        <v>5</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3847,8 +3790,12 @@
       <c r="C45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="D45" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4">
         <v>1</v>
@@ -4405,7 +4352,7 @@
         <v>86</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4">
@@ -4516,7 +4463,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>9</v>
@@ -4533,7 +4480,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>9</v>
@@ -4646,7 +4593,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>3</v>
@@ -4655,7 +4602,7 @@
         <v>85</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>211</v>
@@ -4957,7 +4904,7 @@
         <v>222</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F115" s="4"/>
       <c r="G115" s="4">
@@ -5833,7 +5780,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>3</v>
@@ -5856,7 +5803,7 @@
         <v>9</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -5873,7 +5820,7 @@
         <v>9</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -5890,7 +5837,7 @@
         <v>9</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -5901,7 +5848,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>3</v>
@@ -5924,7 +5871,7 @@
         <v>9</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -5939,7 +5886,7 @@
         <v>9</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -5954,7 +5901,7 @@
         <v>9</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
@@ -5969,7 +5916,7 @@
         <v>9</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
@@ -5984,7 +5931,7 @@
         <v>9</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
@@ -6195,7 +6142,7 @@
         <v>29</v>
       </c>
       <c r="E193" s="14" t="s">
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="F193" s="4"/>
       <c r="G193" s="4">
@@ -6309,7 +6256,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="14" t="s">
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>3</v>
@@ -6318,40 +6265,34 @@
         <v>164</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="E201" s="14" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="F201" s="4"/>
       <c r="G201" s="4">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A202" s="14" t="s">
+      <c r="A202" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C202" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="D202" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E202" s="14" t="s">
-        <v>173</v>
-      </c>
+      <c r="D202" s="4"/>
+      <c r="E202" s="4"/>
       <c r="F202" s="4"/>
-      <c r="G202" s="4">
-        <v>21</v>
-      </c>
+      <c r="G202" s="4"/>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>9</v>
@@ -6366,7 +6307,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>34</v>
+        <v>251</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>9</v>
@@ -6381,7 +6322,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>9</v>
@@ -6395,80 +6336,80 @@
       <c r="G205" s="4"/>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A206" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D206" s="4"/>
-      <c r="E206" s="4"/>
+      <c r="A206" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D206" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E206" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="F206" s="4"/>
-      <c r="G206" s="4"/>
+      <c r="G206" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A207" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="B207" s="2" t="s">
+      <c r="A207" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C207" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D207" s="4"/>
+      <c r="E207" s="4"/>
+      <c r="F207" s="4"/>
+      <c r="G207" s="4"/>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C207" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="D207" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="E207" s="15" t="s">
+      <c r="C208" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D208" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F207" s="4"/>
-      <c r="G207" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A208" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B208" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C208" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D208" s="4"/>
-      <c r="E208" s="4"/>
+      <c r="E208" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="F208" s="4"/>
-      <c r="G208" s="4"/>
+      <c r="G208" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A209" s="15" t="s">
+      <c r="A209" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C209" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D209" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E209" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="D209" s="4"/>
+      <c r="E209" s="4"/>
       <c r="F209" s="4"/>
-      <c r="G209" s="4">
-        <v>2</v>
-      </c>
+      <c r="G209" s="4"/>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A210" s="1" t="s">
-        <v>44</v>
+      <c r="A210" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>9</v>
@@ -6483,7 +6424,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>9</v>
@@ -6497,14 +6438,14 @@
       <c r="G211" s="4"/>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A212" s="15" t="s">
-        <v>46</v>
+      <c r="A212" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C212" s="15" t="s">
-        <v>43</v>
+      <c r="C212" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4"/>
@@ -6512,14 +6453,14 @@
       <c r="G212" s="4"/>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A213" s="1" t="s">
-        <v>52</v>
+      <c r="A213" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C213" s="1" t="s">
-        <v>133</v>
+      <c r="C213" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="D213" s="4"/>
       <c r="E213" s="4"/>
@@ -6527,23 +6468,29 @@
       <c r="G213" s="4"/>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A214" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B214" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C214" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D214" s="4"/>
-      <c r="E214" s="4"/>
+      <c r="A214" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D214" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F214" s="4"/>
-      <c r="G214" s="4"/>
+      <c r="G214" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A215" s="14" t="s">
-        <v>174</v>
+      <c r="A215" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>3</v>
@@ -6551,41 +6498,35 @@
       <c r="C215" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D215" s="14" t="s">
-        <v>174</v>
+      <c r="D215" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="F215" s="4"/>
       <c r="G215" s="4">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B216" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="D216" s="4"/>
+      <c r="E216" s="4"/>
       <c r="F216" s="4"/>
-      <c r="G216" s="4">
-        <v>21</v>
-      </c>
+      <c r="G216" s="4"/>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>253</v>
+        <v>48</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>9</v>
@@ -6600,22 +6541,28 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D218" s="4"/>
-      <c r="E218" s="4"/>
+        <v>175</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F218" s="4"/>
-      <c r="G218" s="4"/>
+      <c r="G218" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>3</v>
@@ -6623,12 +6570,8 @@
       <c r="C219" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D219" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="D219" s="4"/>
+      <c r="E219" s="4"/>
       <c r="F219" s="4"/>
       <c r="G219" s="4">
         <v>1</v>
@@ -6636,392 +6579,370 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4"/>
       <c r="F220" s="4"/>
-      <c r="G220" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A221" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B221" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D221" s="4"/>
-      <c r="E221" s="4"/>
-      <c r="F221" s="4"/>
-      <c r="G221" s="4"/>
+      <c r="G220" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G221" xr:uid="{F728FE19-0465-1C4B-A5E0-C11743CC7188}"/>
+  <autoFilter ref="A1:G220" xr:uid="{F728FE19-0465-1C4B-A5E0-C11743CC7188}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="180" priority="243"/>
-    <cfRule type="duplicateValues" dxfId="179" priority="242"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="249"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="250"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="178" priority="244"/>
-    <cfRule type="duplicateValues" dxfId="177" priority="245"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="251"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="252"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A4">
-    <cfRule type="duplicateValues" dxfId="176" priority="99"/>
-    <cfRule type="duplicateValues" dxfId="175" priority="98"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A14">
-    <cfRule type="duplicateValues" dxfId="174" priority="96"/>
-    <cfRule type="duplicateValues" dxfId="173" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A44">
-    <cfRule type="duplicateValues" dxfId="172" priority="278"/>
-    <cfRule type="duplicateValues" dxfId="171" priority="279"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="285"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="286"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="duplicateValues" dxfId="170" priority="229"/>
-    <cfRule type="duplicateValues" dxfId="169" priority="228"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="235"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="236"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:A52">
-    <cfRule type="duplicateValues" dxfId="168" priority="258"/>
-    <cfRule type="duplicateValues" dxfId="167" priority="259"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="265"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="266"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A80">
-    <cfRule type="duplicateValues" dxfId="166" priority="435"/>
-    <cfRule type="duplicateValues" dxfId="165" priority="434"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="441"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="442"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:A95">
-    <cfRule type="duplicateValues" dxfId="164" priority="169"/>
-    <cfRule type="duplicateValues" dxfId="163" priority="168"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="175"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="176"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="duplicateValues" dxfId="162" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="161" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="duplicateValues" dxfId="160" priority="264"/>
-    <cfRule type="duplicateValues" dxfId="159" priority="265"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="271"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="272"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:A114">
-    <cfRule type="duplicateValues" dxfId="158" priority="167"/>
-    <cfRule type="duplicateValues" dxfId="157" priority="166"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="173"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="174"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
-    <cfRule type="duplicateValues" dxfId="156" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="155" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116 A15:A16 A46:A47 A97 A81">
-    <cfRule type="duplicateValues" dxfId="154" priority="246"/>
-    <cfRule type="duplicateValues" dxfId="153" priority="247"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="253"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="254"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A117 A119">
-    <cfRule type="duplicateValues" dxfId="152" priority="207"/>
-    <cfRule type="duplicateValues" dxfId="151" priority="206"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="213"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118">
-    <cfRule type="duplicateValues" dxfId="150" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="149" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A120:A126">
-    <cfRule type="duplicateValues" dxfId="148" priority="439"/>
-    <cfRule type="duplicateValues" dxfId="147" priority="438"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="445"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="446"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A148">
-    <cfRule type="duplicateValues" dxfId="146" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="145" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150">
-    <cfRule type="duplicateValues" dxfId="144" priority="40"/>
-    <cfRule type="duplicateValues" dxfId="143" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A151 A127:A147 A149">
-    <cfRule type="duplicateValues" dxfId="142" priority="351"/>
-    <cfRule type="duplicateValues" dxfId="141" priority="350"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="357"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="358"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="140" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="139" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154:A155 A158 A160 A162 A164">
-    <cfRule type="duplicateValues" dxfId="138" priority="223"/>
-    <cfRule type="duplicateValues" dxfId="137" priority="222"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="229"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="230"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:A157">
-    <cfRule type="duplicateValues" dxfId="136" priority="161"/>
-    <cfRule type="duplicateValues" dxfId="135" priority="160"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="167"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="168"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A159">
-    <cfRule type="duplicateValues" dxfId="134" priority="159"/>
-    <cfRule type="duplicateValues" dxfId="133" priority="158"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="165"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="166"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A161">
-    <cfRule type="duplicateValues" dxfId="132" priority="156"/>
-    <cfRule type="duplicateValues" dxfId="131" priority="157"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="163"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="164"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A163">
-    <cfRule type="duplicateValues" dxfId="130" priority="155"/>
-    <cfRule type="duplicateValues" dxfId="129" priority="154"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="161"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="162"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A165">
-    <cfRule type="duplicateValues" dxfId="128" priority="152"/>
-    <cfRule type="duplicateValues" dxfId="127" priority="153"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="159"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="160"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A168:A169">
-    <cfRule type="duplicateValues" dxfId="126" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="125" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172:A174">
-    <cfRule type="duplicateValues" dxfId="124" priority="151"/>
-    <cfRule type="duplicateValues" dxfId="123" priority="150"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="157"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="158"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A176:A177 A179:A180">
-    <cfRule type="duplicateValues" dxfId="122" priority="367"/>
-    <cfRule type="duplicateValues" dxfId="121" priority="366"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="373"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="374"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A178">
-    <cfRule type="duplicateValues" dxfId="120" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="119" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182:A186">
-    <cfRule type="duplicateValues" dxfId="118" priority="352"/>
-    <cfRule type="duplicateValues" dxfId="117" priority="353"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="359"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="360"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A187">
-    <cfRule type="duplicateValues" dxfId="116" priority="174"/>
-    <cfRule type="duplicateValues" dxfId="115" priority="175"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="181"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="182"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A188">
-    <cfRule type="duplicateValues" dxfId="114" priority="176"/>
-    <cfRule type="duplicateValues" dxfId="113" priority="177"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="183"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="184"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A189:A192">
-    <cfRule type="duplicateValues" dxfId="112" priority="145"/>
-    <cfRule type="duplicateValues" dxfId="111" priority="144"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="151"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="152"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194:A200">
-    <cfRule type="duplicateValues" dxfId="110" priority="143"/>
-    <cfRule type="duplicateValues" dxfId="109" priority="142"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A201">
-    <cfRule type="duplicateValues" dxfId="108" priority="200"/>
-    <cfRule type="duplicateValues" dxfId="107" priority="201"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A203:A206">
-    <cfRule type="duplicateValues" dxfId="106" priority="141"/>
-    <cfRule type="duplicateValues" dxfId="105" priority="140"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A207">
-    <cfRule type="duplicateValues" dxfId="104" priority="186"/>
-    <cfRule type="duplicateValues" dxfId="103" priority="187"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A213">
-    <cfRule type="duplicateValues" dxfId="102" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="101" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A214 A210:A212">
-    <cfRule type="duplicateValues" dxfId="100" priority="440"/>
-    <cfRule type="duplicateValues" dxfId="99" priority="441"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A215">
-    <cfRule type="duplicateValues" dxfId="98" priority="190"/>
-    <cfRule type="duplicateValues" dxfId="97" priority="191"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A217:A218">
-    <cfRule type="duplicateValues" dxfId="96" priority="442"/>
-    <cfRule type="duplicateValues" dxfId="95" priority="443"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A220 A170:A171 A193 A202 A175 A181 A208:A209">
-    <cfRule type="duplicateValues" dxfId="94" priority="249"/>
-    <cfRule type="duplicateValues" dxfId="93" priority="248"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A221">
-    <cfRule type="duplicateValues" dxfId="92" priority="132"/>
-    <cfRule type="duplicateValues" dxfId="91" priority="133"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="149"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="150"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A202:A205">
+    <cfRule type="duplicateValues" dxfId="103" priority="147"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="148"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A206">
+    <cfRule type="duplicateValues" dxfId="101" priority="193"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="194"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A212">
+    <cfRule type="duplicateValues" dxfId="99" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A213 A209:A211">
+    <cfRule type="duplicateValues" dxfId="97" priority="447"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="448"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A214">
+    <cfRule type="duplicateValues" dxfId="95" priority="197"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="198"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A216:A217">
+    <cfRule type="duplicateValues" dxfId="93" priority="449"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="450"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A219 A170:A171 A193 A201 A175 A181 A207:A208">
+    <cfRule type="duplicateValues" dxfId="91" priority="255"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="256"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A220">
+    <cfRule type="duplicateValues" dxfId="89" priority="139"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="140"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="duplicateValues" dxfId="90" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="89" priority="92"/>
-    <cfRule type="duplicateValues" dxfId="88" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="duplicateValues" dxfId="87" priority="251"/>
-    <cfRule type="duplicateValues" dxfId="86" priority="250"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="257"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="258"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="85" priority="255"/>
-    <cfRule type="duplicateValues" dxfId="84" priority="254"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="261"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="262"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="duplicateValues" dxfId="83" priority="261"/>
-    <cfRule type="duplicateValues" dxfId="82" priority="260"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="267"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="268"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="duplicateValues" dxfId="81" priority="110"/>
-    <cfRule type="duplicateValues" dxfId="80" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="duplicateValues" dxfId="79" priority="268"/>
-    <cfRule type="duplicateValues" dxfId="78" priority="269"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="275"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="276"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D115">
-    <cfRule type="duplicateValues" dxfId="77" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="76" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D117">
+    <cfRule type="duplicateValues" dxfId="72" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D119">
+    <cfRule type="duplicateValues" dxfId="69" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D155">
-    <cfRule type="duplicateValues" dxfId="73" priority="220"/>
-    <cfRule type="duplicateValues" dxfId="72" priority="221"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="227"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="228"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D158">
-    <cfRule type="duplicateValues" dxfId="71" priority="216"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="217"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="223"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="224"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D160">
-    <cfRule type="duplicateValues" dxfId="69" priority="214"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="215"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="221"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="222"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="duplicateValues" dxfId="67" priority="212"/>
-    <cfRule type="duplicateValues" dxfId="66" priority="213"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="219"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="220"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175">
-    <cfRule type="duplicateValues" dxfId="65" priority="101"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="107"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D181">
-    <cfRule type="duplicateValues" dxfId="63" priority="275"/>
-    <cfRule type="duplicateValues" dxfId="62" priority="274"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="281"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="282"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D188">
-    <cfRule type="duplicateValues" dxfId="61" priority="230"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="231"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="237"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="238"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D193">
-    <cfRule type="duplicateValues" dxfId="59" priority="236"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="237"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="243"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="244"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D201">
-    <cfRule type="duplicateValues" dxfId="57" priority="199"/>
-    <cfRule type="duplicateValues" dxfId="56" priority="198"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D202">
-    <cfRule type="duplicateValues" dxfId="55" priority="235"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="234"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D207">
-    <cfRule type="duplicateValues" dxfId="53" priority="205"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="204"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D215">
-    <cfRule type="duplicateValues" dxfId="51" priority="193"/>
-    <cfRule type="duplicateValues" dxfId="50" priority="192"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="241"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="242"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D206">
+    <cfRule type="duplicateValues" dxfId="48" priority="211"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="212"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D214">
+    <cfRule type="duplicateValues" dxfId="46" priority="199"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="200"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="49" priority="95"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="duplicateValues" dxfId="47" priority="127"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="133"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="134"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="duplicateValues" dxfId="45" priority="256"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="257"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="263"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="264"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="duplicateValues" dxfId="43" priority="109"/>
-    <cfRule type="duplicateValues" dxfId="42" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96">
-    <cfRule type="duplicateValues" dxfId="41" priority="107"/>
-    <cfRule type="duplicateValues" dxfId="40" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E98">
-    <cfRule type="duplicateValues" dxfId="39" priority="266"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="267"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="273"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="274"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E115">
-    <cfRule type="duplicateValues" dxfId="37" priority="178"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="179"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="185"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="186"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E117">
+    <cfRule type="duplicateValues" dxfId="30" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E119">
+    <cfRule type="duplicateValues" dxfId="28" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E155">
-    <cfRule type="duplicateValues" dxfId="35" priority="219"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="218"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="225"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="226"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158">
-    <cfRule type="duplicateValues" dxfId="33" priority="210"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="211"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="217"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="218"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E160">
-    <cfRule type="duplicateValues" dxfId="31" priority="208"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="209"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="215"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="216"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E175">
-    <cfRule type="duplicateValues" dxfId="29" priority="105"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E181">
-    <cfRule type="duplicateValues" dxfId="27" priority="277"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="276"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="283"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="284"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E188">
-    <cfRule type="duplicateValues" dxfId="25" priority="232"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="233"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="239"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="240"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E201">
+    <cfRule type="duplicateValues" dxfId="14" priority="191"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="192"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E206">
+    <cfRule type="duplicateValues" dxfId="12" priority="209"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="210"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E208">
+    <cfRule type="duplicateValues" dxfId="10" priority="195"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="196"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E218">
+    <cfRule type="duplicateValues" dxfId="8" priority="189"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="190"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E193">
-    <cfRule type="duplicateValues" dxfId="23" priority="194"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="195"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E201">
-    <cfRule type="duplicateValues" dxfId="21" priority="197"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="196"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E202">
-    <cfRule type="duplicateValues" dxfId="19" priority="185"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="184"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E207">
-    <cfRule type="duplicateValues" dxfId="17" priority="203"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="202"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E209">
-    <cfRule type="duplicateValues" dxfId="15" priority="188"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="189"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E219">
-    <cfRule type="duplicateValues" dxfId="13" priority="183"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="182"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E119">
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D119">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D119">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D117">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D117">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E117">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>